<commit_message>
update indirect method for hait_ehfz
</commit_message>
<xml_diff>
--- a/data/input/post_trddata/20201211/融券公用合约_20201211.xlsx
+++ b/data/input/post_trddata/20201211/融券公用合约_20201211.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\autot0\data\input\post_trddata\20201211\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5859CE-FFC1-432C-AD64-3EDB61EA1168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA01384-3AE7-4A9E-9F60-CD7CB1352CEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="119">
   <si>
     <t>太平洋</t>
   </si>
@@ -383,8 +383,7 @@
     <t>000000026659</t>
   </si>
   <si>
-    <t>600362</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>000000028365</t>
   </si>
 </sst>
 </file>
@@ -715,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3695,8 +3694,59 @@
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B54" s="1" t="s">
+      <c r="A54" t="s">
+        <v>116</v>
+      </c>
+      <c r="B54">
+        <v>600362</v>
+      </c>
+      <c r="C54">
+        <v>20201211</v>
+      </c>
+      <c r="D54">
+        <v>20210611</v>
+      </c>
+      <c r="E54">
+        <v>1000</v>
+      </c>
+      <c r="F54" t="s">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>8.35</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>13.84</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54" t="s">
         <v>118</v>
+      </c>
+      <c r="O54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P54">
+        <v>21040</v>
+      </c>
+      <c r="Q54">
+        <v>1000</v>
+      </c>
+      <c r="R54">
+        <v>21.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>